<commit_message>
Main Charge sheet opens by default
</commit_message>
<xml_diff>
--- a/Prototype - AutoChargeCalcs.xlsx
+++ b/Prototype - AutoChargeCalcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
@@ -1325,6 +1325,12 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1367,12 +1373,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4521,7 +4521,7 @@
   </sheetPr>
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
@@ -4545,15 +4545,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="132" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -5188,35 +5188,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="134" t="str">
+      <c r="A12" s="136" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="135"/>
+      <c r="B12" s="137"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="136" t="str">
+      <c r="D12" s="138" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="137"/>
+      <c r="E12" s="139"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="138" t="str">
+      <c r="G12" s="140" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="139"/>
+      <c r="H12" s="141"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="140" t="str">
+      <c r="J12" s="142" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="141"/>
+      <c r="K12" s="143"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="142" t="str">
+      <c r="M12" s="144" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="143"/>
+      <c r="N12" s="145"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -6050,35 +6050,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="131" t="s">
+      <c r="A32" s="133" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="132"/>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
-      <c r="G32" s="132"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="132"/>
-      <c r="J32" s="132"/>
-      <c r="K32" s="132"/>
-      <c r="L32" s="132"/>
-      <c r="M32" s="132"/>
-      <c r="N32" s="132"/>
-      <c r="O32" s="132"/>
-      <c r="P32" s="132"/>
-      <c r="Q32" s="132"/>
-      <c r="R32" s="132"/>
-      <c r="S32" s="132"/>
-      <c r="T32" s="132"/>
-      <c r="U32" s="132"/>
-      <c r="V32" s="132"/>
-      <c r="W32" s="132"/>
-      <c r="X32" s="132"/>
-      <c r="Y32" s="132"/>
-      <c r="Z32" s="132"/>
-      <c r="AA32" s="133"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="134"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="134"/>
+      <c r="K32" s="134"/>
+      <c r="L32" s="134"/>
+      <c r="M32" s="134"/>
+      <c r="N32" s="134"/>
+      <c r="O32" s="134"/>
+      <c r="P32" s="134"/>
+      <c r="Q32" s="134"/>
+      <c r="R32" s="134"/>
+      <c r="S32" s="134"/>
+      <c r="T32" s="134"/>
+      <c r="U32" s="134"/>
+      <c r="V32" s="134"/>
+      <c r="W32" s="134"/>
+      <c r="X32" s="134"/>
+      <c r="Y32" s="134"/>
+      <c r="Z32" s="134"/>
+      <c r="AA32" s="135"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -7339,7 +7339,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -7375,10 +7375,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="144">
+      <c r="A2" s="130">
         <v>7.6580000000000004</v>
       </c>
-      <c r="B2" s="144">
+      <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
@@ -7398,10 +7398,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="144">
+      <c r="A3" s="130">
         <v>7.7149999999999999</v>
       </c>
-      <c r="B3" s="144">
+      <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
@@ -7417,10 +7417,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="145">
+      <c r="A4" s="131">
         <v>8.9570000000000007</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
@@ -7436,10 +7436,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="144">
+      <c r="A5" s="130">
         <v>9.6129999999999995</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="130">
         <v>1</v>
       </c>
       <c r="C5">
@@ -7448,10 +7448,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="145">
+      <c r="A6" s="131">
         <v>12.506</v>
       </c>
-      <c r="B6" s="144">
+      <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
@@ -7460,10 +7460,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="144">
+      <c r="A7" s="130">
         <v>5.4930000000000003</v>
       </c>
-      <c r="B7" s="144">
+      <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
@@ -7472,10 +7472,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="145">
+      <c r="A8" s="131">
         <v>5.6980000000000004</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
@@ -7484,10 +7484,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="144">
+      <c r="A9" s="130">
         <v>7.7910000000000004</v>
       </c>
-      <c r="B9" s="144">
+      <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
@@ -7496,10 +7496,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="145">
+      <c r="A10" s="131">
         <v>7.8949999999999996</v>
       </c>
-      <c r="B10" s="144">
+      <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
@@ -7508,10 +7508,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="145">
+      <c r="A11" s="131">
         <v>8.5909999999999993</v>
       </c>
-      <c r="B11" s="144">
+      <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
@@ -7520,10 +7520,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="144">
+      <c r="A12" s="130">
         <v>10.977</v>
       </c>
-      <c r="B12" s="144">
+      <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
@@ -7532,10 +7532,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="144">
+      <c r="A13" s="130">
         <v>5.1639999999999997</v>
       </c>
-      <c r="B13" s="144">
+      <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
@@ -7544,10 +7544,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="145">
+      <c r="A14" s="131">
         <v>6.0380000000000003</v>
       </c>
-      <c r="B14" s="144">
+      <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
@@ -7556,10 +7556,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="145">
+      <c r="A15" s="131">
         <v>6.2480000000000002</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
@@ -7568,10 +7568,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="144">
+      <c r="A16" s="130">
         <v>6.3310000000000004</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
@@ -7580,10 +7580,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="130">
         <v>6.8639999999999999</v>
       </c>
-      <c r="B17" s="144">
+      <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
@@ -7592,10 +7592,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="145">
+      <c r="A18" s="131">
         <v>6.8949999999999996</v>
       </c>
-      <c r="B18" s="144">
+      <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
@@ -7604,10 +7604,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="145">
+      <c r="A19" s="131">
         <v>6.9009999999999998</v>
       </c>
-      <c r="B19" s="144">
+      <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
@@ -7616,10 +7616,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="145">
+      <c r="A20" s="131">
         <v>7.1429999999999998</v>
       </c>
-      <c r="B20" s="144">
+      <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
@@ -7628,10 +7628,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="144">
+      <c r="A21" s="130">
         <v>7.16</v>
       </c>
-      <c r="B21" s="144">
+      <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
@@ -7640,10 +7640,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="144">
+      <c r="A22" s="130">
         <v>7.2839999999999998</v>
       </c>
-      <c r="B22" s="144">
+      <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
@@ -7652,10 +7652,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="145">
+      <c r="A23" s="131">
         <v>7.4809999999999999</v>
       </c>
-      <c r="B23" s="144">
+      <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
@@ -7664,10 +7664,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="144">
+      <c r="A24" s="130">
         <v>8.6839999999999993</v>
       </c>
-      <c r="B24" s="144">
+      <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
@@ -7676,10 +7676,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="145">
+      <c r="A25" s="131">
         <v>8.9120000000000008</v>
       </c>
-      <c r="B25" s="144">
+      <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
@@ -7688,8 +7688,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="144"/>
-      <c r="B26" s="144">
+      <c r="A26" s="130"/>
+      <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
@@ -7698,8 +7698,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
-      <c r="B27" s="144">
+      <c r="A27" s="130"/>
+      <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
@@ -7708,8 +7708,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="144"/>
-      <c r="B28" s="144">
+      <c r="A28" s="130"/>
+      <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
@@ -7718,8 +7718,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="144">
+      <c r="A29" s="130"/>
+      <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
@@ -7728,8 +7728,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
-      <c r="B30" s="144">
+      <c r="A30" s="130"/>
+      <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
@@ -7738,8 +7738,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="144">
+      <c r="A31" s="130"/>
+      <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
@@ -7748,8 +7748,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="144">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
         <v>0</v>
       </c>
       <c r="C32">
@@ -7758,8 +7758,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="144">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
         <v>0</v>
       </c>
       <c r="C33">
@@ -7768,8 +7768,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="144">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
         <v>0</v>
       </c>
       <c r="C34">
@@ -7778,8 +7778,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="144">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
         <v>0</v>
       </c>
       <c r="C35">
@@ -7788,8 +7788,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="144">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
         <v>0</v>
       </c>
       <c r="C36">
@@ -7798,8 +7798,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="144">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
         <v>0</v>
       </c>
       <c r="C37">
@@ -7808,8 +7808,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
         <v>0</v>
       </c>
       <c r="C38">
@@ -7818,8 +7818,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="144">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
         <v>0</v>
       </c>
       <c r="C39">
@@ -7828,8 +7828,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
         <v>0</v>
       </c>
       <c r="C40">
@@ -7838,8 +7838,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="144">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
         <v>0</v>
       </c>
       <c r="C41">
@@ -7848,8 +7848,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="144">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
         <v>0</v>
       </c>
       <c r="C42">
@@ -7858,8 +7858,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="144">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
         <v>0</v>
       </c>
       <c r="C43">
@@ -7868,8 +7868,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="144">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
         <v>0</v>
       </c>
       <c r="C44">
@@ -7878,8 +7878,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="144"/>
-      <c r="B45" s="144">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
         <v>0</v>
       </c>
       <c r="C45">
@@ -7888,8 +7888,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="144">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
         <v>0</v>
       </c>
       <c r="C46">
@@ -7898,8 +7898,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="144">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
         <v>0</v>
       </c>
       <c r="C47">
@@ -7908,8 +7908,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="144">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
         <v>0</v>
       </c>
       <c r="C48">
@@ -7918,8 +7918,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="144">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
         <v>0</v>
       </c>
       <c r="C49">
@@ -7928,8 +7928,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="144">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
         <v>0</v>
       </c>
       <c r="C50">
@@ -7938,8 +7938,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="144"/>
-      <c r="B51" s="144">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
         <v>0</v>
       </c>
       <c r="C51">
@@ -8001,10 +8001,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="144">
+      <c r="A2" s="130">
         <v>18.545999999999999</v>
       </c>
-      <c r="B2" s="144">
+      <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
@@ -8024,10 +8024,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="144">
+      <c r="A3" s="130">
         <v>12.461</v>
       </c>
-      <c r="B3" s="144">
+      <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
@@ -8043,10 +8043,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="144">
+      <c r="A4" s="130">
         <v>10.122999999999999</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
@@ -8062,10 +8062,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="144">
+      <c r="A5" s="130">
         <v>6.6609999999999996</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="130">
         <v>1</v>
       </c>
       <c r="C5">
@@ -8074,10 +8074,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="144">
+      <c r="A6" s="130">
         <v>5.5650000000000004</v>
       </c>
-      <c r="B6" s="144">
+      <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
@@ -8086,10 +8086,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="144">
+      <c r="A7" s="130">
         <v>4.3159999999999998</v>
       </c>
-      <c r="B7" s="144">
+      <c r="B7" s="130">
         <v>1</v>
       </c>
       <c r="C7">
@@ -8098,10 +8098,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="144">
+      <c r="A8" s="130">
         <v>29.986999999999998</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
@@ -8110,10 +8110,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="144">
+      <c r="A9" s="130">
         <v>29.632000000000001</v>
       </c>
-      <c r="B9" s="144">
+      <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
@@ -8122,10 +8122,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="144">
+      <c r="A10" s="130">
         <v>28.844000000000001</v>
       </c>
-      <c r="B10" s="144">
+      <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
@@ -8134,10 +8134,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="144">
+      <c r="A11" s="130">
         <v>28.742000000000001</v>
       </c>
-      <c r="B11" s="144">
+      <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
@@ -8146,10 +8146,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="144">
+      <c r="A12" s="130">
         <v>28.638000000000002</v>
       </c>
-      <c r="B12" s="144">
+      <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
@@ -8158,10 +8158,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="144">
+      <c r="A13" s="130">
         <v>28.478999999999999</v>
       </c>
-      <c r="B13" s="144">
+      <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
@@ -8170,10 +8170,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="144">
+      <c r="A14" s="130">
         <v>27.143000000000001</v>
       </c>
-      <c r="B14" s="144">
+      <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
@@ -8182,10 +8182,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="144">
+      <c r="A15" s="130">
         <v>25.873000000000001</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
@@ -8194,10 +8194,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="144">
+      <c r="A16" s="130">
         <v>25.02</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
@@ -8206,10 +8206,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="130">
         <v>24.922999999999998</v>
       </c>
-      <c r="B17" s="144">
+      <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
@@ -8218,10 +8218,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="144">
+      <c r="A18" s="130">
         <v>23.978999999999999</v>
       </c>
-      <c r="B18" s="144">
+      <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
@@ -8230,10 +8230,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="144">
+      <c r="A19" s="130">
         <v>22.062999999999999</v>
       </c>
-      <c r="B19" s="144">
+      <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
@@ -8242,10 +8242,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="144">
+      <c r="A20" s="130">
         <v>21.928000000000001</v>
       </c>
-      <c r="B20" s="144">
+      <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
@@ -8254,10 +8254,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="144">
+      <c r="A21" s="130">
         <v>20.651</v>
       </c>
-      <c r="B21" s="144">
+      <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
@@ -8266,10 +8266,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="144">
+      <c r="A22" s="130">
         <v>20.65</v>
       </c>
-      <c r="B22" s="144">
+      <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
@@ -8278,10 +8278,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="144">
+      <c r="A23" s="130">
         <v>19.782</v>
       </c>
-      <c r="B23" s="144">
+      <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
@@ -8290,10 +8290,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="144">
+      <c r="A24" s="130">
         <v>19.518999999999998</v>
       </c>
-      <c r="B24" s="144">
+      <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
@@ -8302,10 +8302,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="144">
+      <c r="A25" s="130">
         <v>19.449000000000002</v>
       </c>
-      <c r="B25" s="144">
+      <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
@@ -8314,10 +8314,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="144">
+      <c r="A26" s="130">
         <v>15.534000000000001</v>
       </c>
-      <c r="B26" s="144">
+      <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
@@ -8326,10 +8326,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="144">
+      <c r="A27" s="130">
         <v>14.474</v>
       </c>
-      <c r="B27" s="144">
+      <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
@@ -8338,10 +8338,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="144">
+      <c r="A28" s="130">
         <v>11.648999999999999</v>
       </c>
-      <c r="B28" s="144">
+      <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
@@ -8350,10 +8350,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="144">
+      <c r="A29" s="130">
         <v>11.284000000000001</v>
       </c>
-      <c r="B29" s="144">
+      <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
@@ -8362,10 +8362,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="144">
+      <c r="A30" s="130">
         <v>6.8360000000000003</v>
       </c>
-      <c r="B30" s="144">
+      <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
@@ -8374,10 +8374,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="144">
+      <c r="A31" s="130">
         <v>4.4930000000000003</v>
       </c>
-      <c r="B31" s="144">
+      <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
@@ -8386,8 +8386,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="144">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
         <v>0</v>
       </c>
       <c r="C32">
@@ -8396,8 +8396,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="144">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
         <v>0</v>
       </c>
       <c r="C33">
@@ -8406,8 +8406,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="144">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
         <v>0</v>
       </c>
       <c r="C34">
@@ -8416,8 +8416,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="144">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
         <v>0</v>
       </c>
       <c r="C35">
@@ -8426,8 +8426,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="144">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
         <v>0</v>
       </c>
       <c r="C36">
@@ -8436,8 +8436,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="144">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
         <v>0</v>
       </c>
       <c r="C37">
@@ -8446,8 +8446,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
         <v>0</v>
       </c>
       <c r="C38">
@@ -8456,8 +8456,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="144">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
         <v>0</v>
       </c>
       <c r="C39">
@@ -8466,8 +8466,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
         <v>0</v>
       </c>
       <c r="C40">
@@ -8476,8 +8476,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="144">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
         <v>0</v>
       </c>
       <c r="C41">
@@ -8486,8 +8486,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="144">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
         <v>0</v>
       </c>
       <c r="C42">
@@ -8496,8 +8496,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="144">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
         <v>0</v>
       </c>
       <c r="C43">
@@ -8506,8 +8506,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="144">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
         <v>0</v>
       </c>
       <c r="C44">
@@ -8516,8 +8516,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="144"/>
-      <c r="B45" s="144">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
         <v>0</v>
       </c>
       <c r="C45">
@@ -8526,8 +8526,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="144">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
         <v>0</v>
       </c>
       <c r="C46">
@@ -8536,8 +8536,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="144">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
         <v>0</v>
       </c>
       <c r="C47">
@@ -8546,8 +8546,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="144">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
         <v>0</v>
       </c>
       <c r="C48">
@@ -8556,8 +8556,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="144">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
         <v>0</v>
       </c>
       <c r="C49">
@@ -8566,8 +8566,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="144">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
         <v>0</v>
       </c>
       <c r="C50">
@@ -8576,8 +8576,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="144"/>
-      <c r="B51" s="144">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
         <v>0</v>
       </c>
       <c r="C51">
@@ -8639,10 +8639,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="144">
+      <c r="A2" s="130">
         <v>5.85</v>
       </c>
-      <c r="B2" s="144">
+      <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
@@ -8662,10 +8662,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="144">
+      <c r="A3" s="130">
         <v>9.593</v>
       </c>
-      <c r="B3" s="144">
+      <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
@@ -8681,10 +8681,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="144">
+      <c r="A4" s="130">
         <v>9.4710000000000001</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
@@ -8700,10 +8700,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="144">
+      <c r="A5" s="130">
         <v>9.2479999999999993</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
@@ -8712,10 +8712,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="144">
+      <c r="A6" s="130">
         <v>8.4350000000000005</v>
       </c>
-      <c r="B6" s="144">
+      <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
@@ -8724,10 +8724,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="144">
+      <c r="A7" s="130">
         <v>7.6950000000000003</v>
       </c>
-      <c r="B7" s="144">
+      <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
@@ -8736,10 +8736,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="144">
+      <c r="A8" s="130">
         <v>7.4480000000000004</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
@@ -8748,10 +8748,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="144">
+      <c r="A9" s="130">
         <v>6.9880000000000004</v>
       </c>
-      <c r="B9" s="144">
+      <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
@@ -8760,10 +8760,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="144">
+      <c r="A10" s="130">
         <v>6.7270000000000003</v>
       </c>
-      <c r="B10" s="144">
+      <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
@@ -8772,10 +8772,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="144">
+      <c r="A11" s="130">
         <v>5.5860000000000003</v>
       </c>
-      <c r="B11" s="144">
+      <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
@@ -8784,10 +8784,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="144">
+      <c r="A12" s="130">
         <v>5.5129999999999999</v>
       </c>
-      <c r="B12" s="144">
+      <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
@@ -8796,10 +8796,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="144">
+      <c r="A13" s="130">
         <v>5.3840000000000003</v>
       </c>
-      <c r="B13" s="144">
+      <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
@@ -8808,10 +8808,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="144">
+      <c r="A14" s="130">
         <v>5.2220000000000004</v>
       </c>
-      <c r="B14" s="144">
+      <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
@@ -8820,10 +8820,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="144">
+      <c r="A15" s="130">
         <v>4.923</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
@@ -8832,10 +8832,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="144">
+      <c r="A16" s="130">
         <v>4.7759999999999998</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
@@ -8844,10 +8844,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="130">
         <v>4.2690000000000001</v>
       </c>
-      <c r="B17" s="144">
+      <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
@@ -8856,10 +8856,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="144">
+      <c r="A18" s="130">
         <v>4.165</v>
       </c>
-      <c r="B18" s="144">
+      <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
@@ -8868,10 +8868,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="144">
+      <c r="A19" s="130">
         <v>4.1280000000000001</v>
       </c>
-      <c r="B19" s="144">
+      <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
@@ -8880,10 +8880,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="144">
+      <c r="A20" s="130">
         <v>3.9380000000000002</v>
       </c>
-      <c r="B20" s="144">
+      <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
@@ -8892,10 +8892,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="144">
+      <c r="A21" s="130">
         <v>2.4849999999999999</v>
       </c>
-      <c r="B21" s="144">
+      <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
@@ -8904,10 +8904,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="144">
+      <c r="A22" s="130">
         <v>3.2149999999999999</v>
       </c>
-      <c r="B22" s="144">
+      <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
@@ -8916,10 +8916,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="144">
+      <c r="A23" s="130">
         <v>0.42149999999999999</v>
       </c>
-      <c r="B23" s="144">
+      <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
@@ -8928,8 +8928,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
-      <c r="B24" s="144">
+      <c r="A24" s="130"/>
+      <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
@@ -8938,8 +8938,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="144"/>
-      <c r="B25" s="144">
+      <c r="A25" s="130"/>
+      <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
@@ -8948,8 +8948,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="144"/>
-      <c r="B26" s="144">
+      <c r="A26" s="130"/>
+      <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
@@ -8958,8 +8958,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
-      <c r="B27" s="144">
+      <c r="A27" s="130"/>
+      <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
@@ -8968,8 +8968,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="144"/>
-      <c r="B28" s="144">
+      <c r="A28" s="130"/>
+      <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
@@ -8978,8 +8978,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="144">
+      <c r="A29" s="130"/>
+      <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
@@ -8988,8 +8988,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
-      <c r="B30" s="144">
+      <c r="A30" s="130"/>
+      <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
@@ -8998,8 +8998,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="144">
+      <c r="A31" s="130"/>
+      <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
@@ -9008,8 +9008,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="144">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
         <v>0</v>
       </c>
       <c r="C32">
@@ -9018,8 +9018,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="144">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
         <v>0</v>
       </c>
       <c r="C33">
@@ -9028,8 +9028,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="144">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
         <v>0</v>
       </c>
       <c r="C34">
@@ -9038,8 +9038,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="144">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
         <v>0</v>
       </c>
       <c r="C35">
@@ -9048,8 +9048,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="144">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
         <v>0</v>
       </c>
       <c r="C36">
@@ -9058,8 +9058,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="144">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
         <v>0</v>
       </c>
       <c r="C37">
@@ -9068,8 +9068,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
         <v>0</v>
       </c>
       <c r="C38">
@@ -9078,8 +9078,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="144">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
         <v>0</v>
       </c>
       <c r="C39">
@@ -9088,8 +9088,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
         <v>0</v>
       </c>
       <c r="C40">
@@ -9098,8 +9098,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="144">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
         <v>0</v>
       </c>
       <c r="C41">
@@ -9108,8 +9108,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="144">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
         <v>0</v>
       </c>
       <c r="C42">
@@ -9118,8 +9118,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="144">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
         <v>0</v>
       </c>
       <c r="C43">
@@ -9128,8 +9128,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="144">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
         <v>0</v>
       </c>
       <c r="C44">
@@ -9138,8 +9138,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="144"/>
-      <c r="B45" s="144">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
         <v>0</v>
       </c>
       <c r="C45">
@@ -9148,8 +9148,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="144">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
         <v>0</v>
       </c>
       <c r="C46">
@@ -9158,8 +9158,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="144">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
         <v>0</v>
       </c>
       <c r="C47">
@@ -9168,8 +9168,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="144">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
         <v>0</v>
       </c>
       <c r="C48">
@@ -9178,8 +9178,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="144">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
         <v>0</v>
       </c>
       <c r="C49">
@@ -9188,8 +9188,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="144">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
         <v>0</v>
       </c>
       <c r="C50">
@@ -9198,8 +9198,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="144"/>
-      <c r="B51" s="144">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
         <v>0</v>
       </c>
       <c r="C51">
@@ -9261,10 +9261,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="144">
+      <c r="A2" s="130">
         <v>9.1289999999999996</v>
       </c>
-      <c r="B2" s="144">
+      <c r="B2" s="130">
         <v>0</v>
       </c>
       <c r="C2">
@@ -9284,10 +9284,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="144">
+      <c r="A3" s="130">
         <v>0.16300000000000001</v>
       </c>
-      <c r="B3" s="144">
+      <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
@@ -9303,10 +9303,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="144">
+      <c r="A4" s="130">
         <v>1.71</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
@@ -9322,10 +9322,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="144">
+      <c r="A5" s="130">
         <v>3.4380000000000002</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
@@ -9334,10 +9334,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="144">
+      <c r="A6" s="130">
         <v>0.35299999999999998</v>
       </c>
-      <c r="B6" s="144">
+      <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
@@ -9346,10 +9346,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="144">
+      <c r="A7" s="130">
         <v>1.746</v>
       </c>
-      <c r="B7" s="144">
+      <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
@@ -9358,10 +9358,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="144">
+      <c r="A8" s="130">
         <v>7.5640000000000001</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
@@ -9370,10 +9370,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="144">
+      <c r="A9" s="130">
         <v>9.3130000000000006</v>
       </c>
-      <c r="B9" s="144">
+      <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
@@ -9382,10 +9382,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="144">
+      <c r="A10" s="130">
         <v>4.22</v>
       </c>
-      <c r="B10" s="144">
+      <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
@@ -9394,10 +9394,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="144">
+      <c r="A11" s="130">
         <v>3.55</v>
       </c>
-      <c r="B11" s="144">
+      <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
@@ -9406,10 +9406,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="144">
+      <c r="A12" s="130">
         <v>0.67800000000000005</v>
       </c>
-      <c r="B12" s="144">
+      <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
@@ -9418,10 +9418,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="144">
+      <c r="A13" s="130">
         <v>2.1190000000000002</v>
       </c>
-      <c r="B13" s="144">
+      <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
@@ -9430,10 +9430,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="144">
+      <c r="A14" s="130">
         <v>0.106</v>
       </c>
-      <c r="B14" s="144">
+      <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
@@ -9442,10 +9442,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="144">
+      <c r="A15" s="130">
         <v>0.185</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
@@ -9454,10 +9454,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="144">
+      <c r="A16" s="130">
         <v>5.9859999999999998</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
@@ -9466,10 +9466,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="130">
         <v>0.184</v>
       </c>
-      <c r="B17" s="144">
+      <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
@@ -9478,10 +9478,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="144">
+      <c r="A18" s="130">
         <v>1.6379999999999999</v>
       </c>
-      <c r="B18" s="144">
+      <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
@@ -9490,10 +9490,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="144">
+      <c r="A19" s="130">
         <v>7.2069999999999999</v>
       </c>
-      <c r="B19" s="144">
+      <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
@@ -9502,10 +9502,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="144">
+      <c r="A20" s="130">
         <v>2.1840000000000002</v>
       </c>
-      <c r="B20" s="144">
+      <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
@@ -9514,10 +9514,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="144">
+      <c r="A21" s="130">
         <v>1.2290000000000001</v>
       </c>
-      <c r="B21" s="144">
+      <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
@@ -9526,10 +9526,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="144">
+      <c r="A22" s="130">
         <v>0.79400000000000004</v>
       </c>
-      <c r="B22" s="144">
+      <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
@@ -9538,10 +9538,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="144">
+      <c r="A23" s="130">
         <v>8.4559999999999995</v>
       </c>
-      <c r="B23" s="144">
+      <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
@@ -9550,10 +9550,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="144">
+      <c r="A24" s="130">
         <v>8.8759999999999994</v>
       </c>
-      <c r="B24" s="144">
+      <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
@@ -9562,10 +9562,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="144">
+      <c r="A25" s="130">
         <v>9.8610000000000007</v>
       </c>
-      <c r="B25" s="144">
+      <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
@@ -9574,10 +9574,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="144">
+      <c r="A26" s="130">
         <v>8.5350000000000001</v>
       </c>
-      <c r="B26" s="144">
+      <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
@@ -9586,10 +9586,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="144">
+      <c r="A27" s="130">
         <v>2.1269999999999998</v>
       </c>
-      <c r="B27" s="144">
+      <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
@@ -9598,10 +9598,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="144">
+      <c r="A28" s="130">
         <v>1.4039999999999999</v>
       </c>
-      <c r="B28" s="144">
+      <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
@@ -9610,8 +9610,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="144">
+      <c r="A29" s="130"/>
+      <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
@@ -9620,8 +9620,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
-      <c r="B30" s="144">
+      <c r="A30" s="130"/>
+      <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
@@ -9630,8 +9630,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="144">
+      <c r="A31" s="130"/>
+      <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
@@ -9640,8 +9640,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="144">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
         <v>0</v>
       </c>
       <c r="C32">
@@ -9650,8 +9650,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="144">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
         <v>0</v>
       </c>
       <c r="C33">
@@ -9660,8 +9660,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="144">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
         <v>0</v>
       </c>
       <c r="C34">
@@ -9670,8 +9670,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="144">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
         <v>0</v>
       </c>
       <c r="C35">
@@ -9680,8 +9680,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="144">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
         <v>0</v>
       </c>
       <c r="C36">
@@ -9690,8 +9690,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="144">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
         <v>0</v>
       </c>
       <c r="C37">
@@ -9700,8 +9700,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
         <v>0</v>
       </c>
       <c r="C38">
@@ -9710,8 +9710,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="144">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
         <v>0</v>
       </c>
       <c r="C39">
@@ -9720,8 +9720,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
         <v>0</v>
       </c>
       <c r="C40">
@@ -9730,8 +9730,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="144">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
         <v>0</v>
       </c>
       <c r="C41">
@@ -9740,8 +9740,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="144">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
         <v>0</v>
       </c>
       <c r="C42">
@@ -9750,8 +9750,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="144">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
         <v>0</v>
       </c>
       <c r="C43">
@@ -9760,8 +9760,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="144">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
         <v>0</v>
       </c>
       <c r="C44">
@@ -9770,8 +9770,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="144"/>
-      <c r="B45" s="144">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
         <v>0</v>
       </c>
       <c r="C45">
@@ -9780,8 +9780,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="144">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
         <v>0</v>
       </c>
       <c r="C46">
@@ -9790,8 +9790,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="144">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
         <v>0</v>
       </c>
       <c r="C47">
@@ -9800,8 +9800,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="144">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
         <v>0</v>
       </c>
       <c r="C48">
@@ -9810,8 +9810,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="144">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
         <v>0</v>
       </c>
       <c r="C49">
@@ -9820,8 +9820,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="144">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
         <v>0</v>
       </c>
       <c r="C50">
@@ -9830,8 +9830,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="144"/>
-      <c r="B51" s="144">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
         <v>0</v>
       </c>
       <c r="C51">
@@ -9893,10 +9893,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="144">
+      <c r="A2" s="130">
         <v>4.1269999999999998</v>
       </c>
-      <c r="B2" s="144">
+      <c r="B2" s="130">
         <v>0</v>
       </c>
       <c r="C2">
@@ -9916,10 +9916,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="144">
+      <c r="A3" s="130">
         <v>5.1159999999999997</v>
       </c>
-      <c r="B3" s="144">
+      <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
@@ -9935,10 +9935,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="144">
+      <c r="A4" s="130">
         <v>5.7830000000000004</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
@@ -9954,10 +9954,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="144">
+      <c r="A5" s="130">
         <v>2.669</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
@@ -9966,10 +9966,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="144">
+      <c r="A6" s="130">
         <v>6.3630000000000004</v>
       </c>
-      <c r="B6" s="144">
+      <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
@@ -9978,10 +9978,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="144">
+      <c r="A7" s="130">
         <v>1.627</v>
       </c>
-      <c r="B7" s="144">
+      <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
@@ -9990,10 +9990,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="144">
+      <c r="A8" s="130">
         <v>2.1080000000000001</v>
       </c>
-      <c r="B8" s="144">
+      <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
@@ -10002,10 +10002,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="144">
+      <c r="A9" s="130">
         <v>1.4119999999999999</v>
       </c>
-      <c r="B9" s="144">
+      <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
@@ -10014,10 +10014,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="144">
+      <c r="A10" s="130">
         <v>8.0530000000000008</v>
       </c>
-      <c r="B10" s="144">
+      <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
@@ -10026,10 +10026,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="144">
+      <c r="A11" s="130">
         <v>3.8090000000000002</v>
       </c>
-      <c r="B11" s="144">
+      <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
@@ -10038,10 +10038,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="144">
+      <c r="A12" s="130">
         <v>2.6139999999999999</v>
       </c>
-      <c r="B12" s="144">
+      <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
@@ -10050,10 +10050,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="144">
+      <c r="A13" s="130">
         <v>3.5190000000000001</v>
       </c>
-      <c r="B13" s="144">
+      <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
@@ -10062,10 +10062,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="144">
+      <c r="A14" s="130">
         <v>8.4550000000000001</v>
       </c>
-      <c r="B14" s="144">
+      <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
@@ -10074,10 +10074,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="144">
+      <c r="A15" s="130">
         <v>5.8879999999999999</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
@@ -10086,10 +10086,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="144">
+      <c r="A16" s="130">
         <v>8.1110000000000007</v>
       </c>
-      <c r="B16" s="144">
+      <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
@@ -10098,10 +10098,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="130">
         <v>5.0190000000000001</v>
       </c>
-      <c r="B17" s="144">
+      <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
@@ -10110,10 +10110,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="144">
+      <c r="A18" s="130">
         <v>7.85</v>
       </c>
-      <c r="B18" s="144">
+      <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
@@ -10122,10 +10122,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="144">
+      <c r="A19" s="130">
         <v>4.3769999999999998</v>
       </c>
-      <c r="B19" s="144">
+      <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
@@ -10134,10 +10134,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="144">
+      <c r="A20" s="130">
         <v>6.49</v>
       </c>
-      <c r="B20" s="144">
+      <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
@@ -10146,10 +10146,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="144">
+      <c r="A21" s="130">
         <v>7.4050000000000002</v>
       </c>
-      <c r="B21" s="144">
+      <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
@@ -10158,10 +10158,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="144">
+      <c r="A22" s="130">
         <v>2.8319999999999999</v>
       </c>
-      <c r="B22" s="144">
+      <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
@@ -10170,10 +10170,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="144">
+      <c r="A23" s="130">
         <v>3.2509999999999999</v>
       </c>
-      <c r="B23" s="144">
+      <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
@@ -10182,10 +10182,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="144">
+      <c r="A24" s="130">
         <v>3.2069999999999999</v>
       </c>
-      <c r="B24" s="144">
+      <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
@@ -10194,10 +10194,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="144">
+      <c r="A25" s="130">
         <v>8.4109999999999996</v>
       </c>
-      <c r="B25" s="144">
+      <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
@@ -10206,10 +10206,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="144">
+      <c r="A26" s="130">
         <v>4.9119999999999999</v>
       </c>
-      <c r="B26" s="144">
+      <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
@@ -10218,10 +10218,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="144">
+      <c r="A27" s="130">
         <v>7.851</v>
       </c>
-      <c r="B27" s="144">
+      <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
@@ -10230,10 +10230,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="144">
+      <c r="A28" s="130">
         <v>4.3890000000000002</v>
       </c>
-      <c r="B28" s="144">
+      <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
@@ -10242,8 +10242,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="144">
+      <c r="A29" s="130"/>
+      <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
@@ -10252,8 +10252,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
-      <c r="B30" s="144">
+      <c r="A30" s="130"/>
+      <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
@@ -10262,8 +10262,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="144">
+      <c r="A31" s="130"/>
+      <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
@@ -10272,8 +10272,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="144">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
         <v>0</v>
       </c>
       <c r="C32">
@@ -10282,8 +10282,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="144">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
         <v>0</v>
       </c>
       <c r="C33">
@@ -10292,8 +10292,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="144">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
         <v>0</v>
       </c>
       <c r="C34">
@@ -10302,8 +10302,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="144">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
         <v>0</v>
       </c>
       <c r="C35">
@@ -10312,8 +10312,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="144">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
         <v>0</v>
       </c>
       <c r="C36">
@@ -10322,8 +10322,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="144">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
         <v>0</v>
       </c>
       <c r="C37">
@@ -10332,8 +10332,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
         <v>0</v>
       </c>
       <c r="C38">
@@ -10342,8 +10342,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="144">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
         <v>0</v>
       </c>
       <c r="C39">
@@ -10352,8 +10352,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
         <v>0</v>
       </c>
       <c r="C40">
@@ -10362,8 +10362,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="144">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
         <v>0</v>
       </c>
       <c r="C41">
@@ -10372,8 +10372,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="144">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
         <v>0</v>
       </c>
       <c r="C42">
@@ -10382,8 +10382,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="144">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
         <v>0</v>
       </c>
       <c r="C43">
@@ -10392,8 +10392,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="144">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
         <v>0</v>
       </c>
       <c r="C44">
@@ -10402,8 +10402,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="144"/>
-      <c r="B45" s="144">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
         <v>0</v>
       </c>
       <c r="C45">
@@ -10412,8 +10412,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="144">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
         <v>0</v>
       </c>
       <c r="C46">
@@ -10422,8 +10422,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="144">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
         <v>0</v>
       </c>
       <c r="C47">
@@ -10432,8 +10432,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="144">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
         <v>0</v>
       </c>
       <c r="C48">
@@ -10442,8 +10442,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="144">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
         <v>0</v>
       </c>
       <c r="C49">
@@ -10452,8 +10452,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="144">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
         <v>0</v>
       </c>
       <c r="C50">
@@ -10462,8 +10462,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="144"/>
-      <c r="B51" s="144">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
         <v>0</v>
       </c>
       <c r="C51">

</xml_diff>

<commit_message>
finished debugging auto-sort sheets
</commit_message>
<xml_diff>
--- a/Prototype - AutoChargeCalcs.xlsx
+++ b/Prototype - AutoChargeCalcs.xlsx
@@ -1080,7 +1080,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1331,6 +1331,7 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1373,6 +1374,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4545,15 +4554,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -4665,11 +4674,11 @@
       </c>
       <c r="F4" s="71">
         <f>ROUND(E4*$F$9, 3)</f>
-        <v>46.445</v>
+        <v>42.222000000000001</v>
       </c>
       <c r="G4" s="72">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>26.723245109321059</v>
+        <v>24.293440736478711</v>
       </c>
       <c r="I4" s="73" t="str">
         <f>$Q$4</f>
@@ -4678,19 +4687,19 @@
       <c r="J4" s="28"/>
       <c r="K4" s="74">
         <f>B29</f>
-        <v>46.448999999999998</v>
+        <v>42.224999999999994</v>
       </c>
       <c r="L4" s="75">
         <f>K4/$K$9</f>
-        <v>0.4223749897700303</v>
+        <v>0.42018688240737978</v>
       </c>
       <c r="M4" s="25">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.7378111078791621E-2</v>
+        <v>1.7288084032395793E-2</v>
       </c>
       <c r="N4" s="120">
         <f>M4/$M$9</f>
-        <v>0.65022215284789109</v>
+        <v>0.64704980052908057</v>
       </c>
       <c r="P4" s="17">
         <v>1</v>
@@ -4758,11 +4767,11 @@
       </c>
       <c r="F5" s="71">
         <f>ROUND(E5*$F$9, 3)</f>
-        <v>57.664000000000001</v>
+        <v>52.421999999999997</v>
       </c>
       <c r="G5" s="72">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>8.0761904761904759</v>
+        <v>7.3420168067226887</v>
       </c>
       <c r="I5" s="73" t="str">
         <f>$Q$5</f>
@@ -4771,19 +4780,19 @@
       <c r="J5" s="29"/>
       <c r="K5" s="77">
         <f>E29</f>
-        <v>57.671999999999997</v>
+        <v>52.415999999999997</v>
       </c>
       <c r="L5" s="78">
         <f>K5/$K$9</f>
-        <v>0.52442916768966363</v>
+        <v>0.52159894915962624</v>
       </c>
       <c r="M5" s="26">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>8.0210022282839865E-3</v>
+        <v>7.9777148016216427E-3</v>
       </c>
       <c r="N5" s="121">
         <f>M5/$M$9</f>
-        <v>0.30011508806831716</v>
+        <v>0.29858593707632664</v>
       </c>
       <c r="P5" s="17">
         <v>2</v>
@@ -4851,11 +4860,11 @@
       </c>
       <c r="F6" s="71">
         <f>ROUND(E6*$F$9, 3)</f>
-        <v>5.891</v>
+        <v>5.3559999999999999</v>
       </c>
       <c r="G6" s="72">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>3.8006451612903223</v>
+        <v>3.4554838709677416</v>
       </c>
       <c r="I6" s="73" t="str">
         <f>$Q$6</f>
@@ -4868,15 +4877,15 @@
       </c>
       <c r="L6" s="78">
         <f>K6/$K$9</f>
-        <v>5.3195842540306085E-2</v>
+        <v>5.8214168432994005E-2</v>
       </c>
       <c r="M6" s="26">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.327307813271772E-3</v>
+        <v>1.4525217933278607E-3</v>
       </c>
       <c r="N6" s="121">
         <f>M6/$M$9</f>
-        <v>4.9662759083791613E-2</v>
+        <v>5.4364262394592786E-2</v>
       </c>
       <c r="P6" s="17">
         <v>3</v>
@@ -5128,11 +5137,11 @@
         <v>1</v>
       </c>
       <c r="F9" s="7">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G9" s="119">
         <f>SUM(G4:G8)</f>
-        <v>38.600080746801851</v>
+        <v>35.090941414169144</v>
       </c>
       <c r="I9" s="85"/>
       <c r="J9" s="81" t="s">
@@ -5140,7 +5149,7 @@
       </c>
       <c r="K9" s="122">
         <f>SUM(K4:K8)</f>
-        <v>109.97099999999999</v>
+        <v>100.49099999999999</v>
       </c>
       <c r="L9" s="86">
         <f>SUM(L4:L8)</f>
@@ -5148,11 +5157,11 @@
       </c>
       <c r="M9" s="123">
         <f>SUM(M4:M8)</f>
-        <v>2.6726421120347382E-2</v>
+        <v>2.6718320627345298E-2</v>
       </c>
       <c r="N9" s="87">
         <f>SUM(N4:N8)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>111</v>
@@ -5188,35 +5197,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="str">
+      <c r="A12" s="137" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="137"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="138" t="str">
+      <c r="D12" s="139" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="139"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="140" t="str">
+      <c r="G12" s="141" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="141"/>
+      <c r="H12" s="142"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="142" t="str">
+      <c r="J12" s="143" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="143"/>
+      <c r="K12" s="144"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="144" t="str">
+      <c r="M12" s="145" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="145"/>
+      <c r="N12" s="146"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -5277,23 +5286,23 @@
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="A14" s="132">
         <v>1</v>
       </c>
       <c r="B14" s="110">
         <f>A!C2</f>
-        <v>7.6580000000000004</v>
+        <v>7.4809999999999999</v>
       </c>
       <c r="C14" s="111"/>
-      <c r="D14" s="29">
+      <c r="D14" s="132">
         <v>1</v>
       </c>
       <c r="E14" s="110">
         <f>B!C2</f>
-        <v>18.545999999999999</v>
+        <v>5.5650000000000004</v>
       </c>
       <c r="F14" s="111"/>
-      <c r="G14" s="29">
+      <c r="G14" s="132">
         <v>1</v>
       </c>
       <c r="H14" s="110">
@@ -5301,7 +5310,7 @@
         <v>5.85</v>
       </c>
       <c r="I14" s="111"/>
-      <c r="J14" s="29">
+      <c r="J14" s="132">
         <v>1</v>
       </c>
       <c r="K14" s="110">
@@ -5309,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="111"/>
-      <c r="M14" s="29">
+      <c r="M14" s="132">
         <v>1</v>
       </c>
       <c r="N14" s="110">
@@ -5327,23 +5336,23 @@
       <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="A15" s="132">
         <v>2</v>
       </c>
       <c r="B15" s="110">
         <f>A!C3</f>
-        <v>7.7149999999999999</v>
+        <v>7.7910000000000004</v>
       </c>
       <c r="C15" s="111"/>
-      <c r="D15" s="29">
+      <c r="D15" s="132">
         <v>2</v>
       </c>
       <c r="E15" s="110">
         <f>B!C3</f>
-        <v>12.461</v>
+        <v>24.922999999999998</v>
       </c>
       <c r="F15" s="111"/>
-      <c r="G15" s="29">
+      <c r="G15" s="132">
         <v>2</v>
       </c>
       <c r="H15" s="110">
@@ -5351,7 +5360,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="111"/>
-      <c r="J15" s="29">
+      <c r="J15" s="132">
         <v>2</v>
       </c>
       <c r="K15" s="110">
@@ -5359,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="111"/>
-      <c r="M15" s="29">
+      <c r="M15" s="132">
         <v>2</v>
       </c>
       <c r="N15" s="110">
@@ -5377,23 +5386,23 @@
       <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="A16" s="132">
         <v>3</v>
       </c>
       <c r="B16" s="110">
         <f>A!C4</f>
-        <v>8.9570000000000007</v>
+        <v>8.5909999999999993</v>
       </c>
       <c r="C16" s="111"/>
-      <c r="D16" s="29">
+      <c r="D16" s="132">
         <v>3</v>
       </c>
       <c r="E16" s="110">
         <f>B!C4</f>
-        <v>10.122999999999999</v>
+        <v>21.928000000000001</v>
       </c>
       <c r="F16" s="111"/>
-      <c r="G16" s="29">
+      <c r="G16" s="132">
         <v>3</v>
       </c>
       <c r="H16" s="110">
@@ -5401,7 +5410,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="111"/>
-      <c r="J16" s="29">
+      <c r="J16" s="132">
         <v>3</v>
       </c>
       <c r="K16" s="110">
@@ -5409,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="111"/>
-      <c r="M16" s="29">
+      <c r="M16" s="132">
         <v>3</v>
       </c>
       <c r="N16" s="110">
@@ -5427,23 +5436,23 @@
       <c r="T16" s="9"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="A17" s="132">
         <v>4</v>
       </c>
       <c r="B17" s="110">
         <f>A!C5</f>
-        <v>9.6129999999999995</v>
+        <v>5.1639999999999997</v>
       </c>
       <c r="C17" s="111"/>
-      <c r="D17" s="29">
+      <c r="D17" s="132">
         <v>4</v>
       </c>
       <c r="E17" s="110">
         <f>B!C5</f>
-        <v>6.6609999999999996</v>
+        <v>0</v>
       </c>
       <c r="F17" s="111"/>
-      <c r="G17" s="29">
+      <c r="G17" s="132">
         <v>4</v>
       </c>
       <c r="H17" s="110">
@@ -5451,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="111"/>
-      <c r="J17" s="29">
+      <c r="J17" s="132">
         <v>4</v>
       </c>
       <c r="K17" s="110">
@@ -5459,7 +5468,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="111"/>
-      <c r="M17" s="29">
+      <c r="M17" s="132">
         <v>4</v>
       </c>
       <c r="N17" s="110">
@@ -5477,23 +5486,23 @@
       <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="132">
         <v>5</v>
       </c>
       <c r="B18" s="110">
         <f>A!C6</f>
-        <v>12.506</v>
+        <v>6.0380000000000003</v>
       </c>
       <c r="C18" s="111"/>
-      <c r="D18" s="29">
+      <c r="D18" s="132">
         <v>5</v>
       </c>
       <c r="E18" s="110">
         <f>B!C6</f>
-        <v>5.5650000000000004</v>
+        <v>0</v>
       </c>
       <c r="F18" s="111"/>
-      <c r="G18" s="29">
+      <c r="G18" s="132">
         <v>5</v>
       </c>
       <c r="H18" s="110">
@@ -5501,7 +5510,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="111"/>
-      <c r="J18" s="29">
+      <c r="J18" s="132">
         <v>5</v>
       </c>
       <c r="K18" s="110">
@@ -5509,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="111"/>
-      <c r="M18" s="29">
+      <c r="M18" s="132">
         <v>5</v>
       </c>
       <c r="N18" s="110">
@@ -5529,23 +5538,23 @@
       <c r="T18" s="9"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="132">
         <v>6</v>
       </c>
       <c r="B19" s="110">
         <f>A!C7</f>
-        <v>0</v>
+        <v>7.16</v>
       </c>
       <c r="C19" s="111"/>
-      <c r="D19" s="29">
+      <c r="D19" s="132">
         <v>6</v>
       </c>
       <c r="E19" s="110">
         <f>B!C7</f>
-        <v>4.3159999999999998</v>
+        <v>0</v>
       </c>
       <c r="F19" s="111"/>
-      <c r="G19" s="29">
+      <c r="G19" s="132">
         <v>6</v>
       </c>
       <c r="H19" s="110">
@@ -5553,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="111"/>
-      <c r="J19" s="29">
+      <c r="J19" s="132">
         <v>6</v>
       </c>
       <c r="K19" s="110">
@@ -5561,7 +5570,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="111"/>
-      <c r="M19" s="29">
+      <c r="M19" s="132">
         <v>6</v>
       </c>
       <c r="N19" s="110">
@@ -5577,7 +5586,7 @@
       <c r="T19" s="9"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="132">
         <v>7</v>
       </c>
       <c r="B20" s="110">
@@ -5585,7 +5594,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="111"/>
-      <c r="D20" s="29">
+      <c r="D20" s="132">
         <v>7</v>
       </c>
       <c r="E20" s="110">
@@ -5593,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="111"/>
-      <c r="G20" s="29">
+      <c r="G20" s="132">
         <v>7</v>
       </c>
       <c r="H20" s="110">
@@ -5601,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="111"/>
-      <c r="J20" s="29">
+      <c r="J20" s="132">
         <v>7</v>
       </c>
       <c r="K20" s="110">
@@ -5609,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="111"/>
-      <c r="M20" s="29">
+      <c r="M20" s="132">
         <v>7</v>
       </c>
       <c r="N20" s="110">
@@ -5625,7 +5634,7 @@
       <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="132">
         <v>8</v>
       </c>
       <c r="B21" s="110">
@@ -5633,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="111"/>
-      <c r="D21" s="29">
+      <c r="D21" s="132">
         <v>8</v>
       </c>
       <c r="E21" s="110">
@@ -5641,7 +5650,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="111"/>
-      <c r="G21" s="29">
+      <c r="G21" s="132">
         <v>8</v>
       </c>
       <c r="H21" s="110">
@@ -5649,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="111"/>
-      <c r="J21" s="29">
+      <c r="J21" s="132">
         <v>8</v>
       </c>
       <c r="K21" s="110">
@@ -5657,7 +5666,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="111"/>
-      <c r="M21" s="29">
+      <c r="M21" s="132">
         <v>8</v>
       </c>
       <c r="N21" s="110">
@@ -5673,7 +5682,7 @@
       <c r="T21" s="9"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="132">
         <v>9</v>
       </c>
       <c r="B22" s="110">
@@ -5681,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="111"/>
-      <c r="D22" s="29">
+      <c r="D22" s="132">
         <v>9</v>
       </c>
       <c r="E22" s="110">
@@ -5689,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="111"/>
-      <c r="G22" s="29">
+      <c r="G22" s="132">
         <v>9</v>
       </c>
       <c r="H22" s="110">
@@ -5697,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="111"/>
-      <c r="J22" s="29">
+      <c r="J22" s="132">
         <v>9</v>
       </c>
       <c r="K22" s="110">
@@ -5705,7 +5714,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="111"/>
-      <c r="M22" s="29">
+      <c r="M22" s="132">
         <v>9</v>
       </c>
       <c r="N22" s="110">
@@ -5721,7 +5730,7 @@
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="132">
         <v>10</v>
       </c>
       <c r="B23" s="110">
@@ -5729,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="111"/>
-      <c r="D23" s="29">
+      <c r="D23" s="132">
         <v>10</v>
       </c>
       <c r="E23" s="110">
@@ -5737,7 +5746,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="111"/>
-      <c r="G23" s="29">
+      <c r="G23" s="132">
         <v>10</v>
       </c>
       <c r="H23" s="110">
@@ -5745,7 +5754,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="111"/>
-      <c r="J23" s="29">
+      <c r="J23" s="132">
         <v>10</v>
       </c>
       <c r="K23" s="110">
@@ -5753,7 +5762,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="111"/>
-      <c r="M23" s="29">
+      <c r="M23" s="132">
         <v>10</v>
       </c>
       <c r="N23" s="110">
@@ -5762,7 +5771,7 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
+      <c r="A24" s="132">
         <v>11</v>
       </c>
       <c r="B24" s="110">
@@ -5770,7 +5779,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="111"/>
-      <c r="D24" s="29">
+      <c r="D24" s="132">
         <v>11</v>
       </c>
       <c r="E24" s="110">
@@ -5778,7 +5787,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="111"/>
-      <c r="G24" s="29">
+      <c r="G24" s="132">
         <v>11</v>
       </c>
       <c r="H24" s="110">
@@ -5786,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="111"/>
-      <c r="J24" s="29">
+      <c r="J24" s="132">
         <v>11</v>
       </c>
       <c r="K24" s="110">
@@ -5794,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="111"/>
-      <c r="M24" s="29">
+      <c r="M24" s="132">
         <v>11</v>
       </c>
       <c r="N24" s="110">
@@ -5803,7 +5812,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="132">
         <v>12</v>
       </c>
       <c r="B25" s="110">
@@ -5811,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="111"/>
-      <c r="D25" s="29">
+      <c r="D25" s="132">
         <v>12</v>
       </c>
       <c r="E25" s="110">
@@ -5819,7 +5828,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="111"/>
-      <c r="G25" s="29">
+      <c r="G25" s="132">
         <v>12</v>
       </c>
       <c r="H25" s="110">
@@ -5827,7 +5836,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="111"/>
-      <c r="J25" s="29">
+      <c r="J25" s="132">
         <v>12</v>
       </c>
       <c r="K25" s="110">
@@ -5835,7 +5844,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="111"/>
-      <c r="M25" s="29">
+      <c r="M25" s="132">
         <v>12</v>
       </c>
       <c r="N25" s="110">
@@ -5844,7 +5853,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
+      <c r="A26" s="132">
         <v>13</v>
       </c>
       <c r="B26" s="110">
@@ -5852,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="111"/>
-      <c r="D26" s="29">
+      <c r="D26" s="132">
         <v>13</v>
       </c>
       <c r="E26" s="110">
@@ -5860,7 +5869,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="111"/>
-      <c r="G26" s="29">
+      <c r="G26" s="132">
         <v>13</v>
       </c>
       <c r="H26" s="110">
@@ -5868,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="111"/>
-      <c r="J26" s="29">
+      <c r="J26" s="132">
         <v>13</v>
       </c>
       <c r="K26" s="110">
@@ -5876,7 +5885,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="111"/>
-      <c r="M26" s="29">
+      <c r="M26" s="132">
         <v>13</v>
       </c>
       <c r="N26" s="110">
@@ -5885,7 +5894,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
+      <c r="A27" s="132">
         <v>14</v>
       </c>
       <c r="B27" s="110">
@@ -5893,7 +5902,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="111"/>
-      <c r="D27" s="29">
+      <c r="D27" s="132">
         <v>14</v>
       </c>
       <c r="E27" s="110">
@@ -5901,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="111"/>
-      <c r="G27" s="29">
+      <c r="G27" s="132">
         <v>14</v>
       </c>
       <c r="H27" s="110">
@@ -5909,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="111"/>
-      <c r="J27" s="29">
+      <c r="J27" s="132">
         <v>14</v>
       </c>
       <c r="K27" s="110">
@@ -5917,7 +5926,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="111"/>
-      <c r="M27" s="29">
+      <c r="M27" s="132">
         <v>14</v>
       </c>
       <c r="N27" s="110">
@@ -5926,7 +5935,7 @@
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
+      <c r="A28" s="132">
         <v>15</v>
       </c>
       <c r="B28" s="110">
@@ -5934,7 +5943,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="111"/>
-      <c r="D28" s="29">
+      <c r="D28" s="132">
         <v>15</v>
       </c>
       <c r="E28" s="110">
@@ -5942,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="111"/>
-      <c r="G28" s="29">
+      <c r="G28" s="132">
         <v>15</v>
       </c>
       <c r="H28" s="110">
@@ -5950,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="111"/>
-      <c r="J28" s="29">
+      <c r="J28" s="132">
         <v>15</v>
       </c>
       <c r="K28" s="110">
@@ -5958,7 +5967,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="111"/>
-      <c r="M28" s="29">
+      <c r="M28" s="132">
         <v>15</v>
       </c>
       <c r="N28" s="110">
@@ -5972,7 +5981,7 @@
       </c>
       <c r="B29" s="114">
         <f>SUM(B14:B28)</f>
-        <v>46.448999999999998</v>
+        <v>42.224999999999994</v>
       </c>
       <c r="C29" s="111"/>
       <c r="D29" s="113" t="s">
@@ -5980,7 +5989,7 @@
       </c>
       <c r="E29" s="115">
         <f>SUM(E14:E28)</f>
-        <v>57.671999999999997</v>
+        <v>52.415999999999997</v>
       </c>
       <c r="F29" s="111"/>
       <c r="G29" s="113" t="s">
@@ -6013,7 +6022,7 @@
       </c>
       <c r="B30" s="117">
         <f>B29-$F$4</f>
-        <v>3.9999999999977831E-3</v>
+        <v>2.9999999999930083E-3</v>
       </c>
       <c r="C30" s="118"/>
       <c r="D30" s="116" t="s">
@@ -6021,7 +6030,7 @@
       </c>
       <c r="E30" s="117">
         <f>E29-$F$5</f>
-        <v>7.9999999999955662E-3</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
       <c r="F30" s="118"/>
       <c r="G30" s="116" t="s">
@@ -6029,7 +6038,7 @@
       </c>
       <c r="H30" s="117">
         <f>H29-$F$6</f>
-        <v>-4.1000000000000369E-2</v>
+        <v>0.49399999999999977</v>
       </c>
       <c r="I30" s="118"/>
       <c r="J30" s="116" t="s">
@@ -6050,35 +6059,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="133" t="s">
+      <c r="A32" s="134" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="134"/>
-      <c r="I32" s="134"/>
-      <c r="J32" s="134"/>
-      <c r="K32" s="134"/>
-      <c r="L32" s="134"/>
-      <c r="M32" s="134"/>
-      <c r="N32" s="134"/>
-      <c r="O32" s="134"/>
-      <c r="P32" s="134"/>
-      <c r="Q32" s="134"/>
-      <c r="R32" s="134"/>
-      <c r="S32" s="134"/>
-      <c r="T32" s="134"/>
-      <c r="U32" s="134"/>
-      <c r="V32" s="134"/>
-      <c r="W32" s="134"/>
-      <c r="X32" s="134"/>
-      <c r="Y32" s="134"/>
-      <c r="Z32" s="134"/>
-      <c r="AA32" s="135"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="135"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="135"/>
+      <c r="N32" s="135"/>
+      <c r="O32" s="135"/>
+      <c r="P32" s="135"/>
+      <c r="Q32" s="135"/>
+      <c r="R32" s="135"/>
+      <c r="S32" s="135"/>
+      <c r="T32" s="135"/>
+      <c r="U32" s="135"/>
+      <c r="V32" s="135"/>
+      <c r="W32" s="135"/>
+      <c r="X32" s="135"/>
+      <c r="Y32" s="135"/>
+      <c r="Z32" s="135"/>
+      <c r="AA32" s="136"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -7346,10 +7355,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -7364,302 +7373,304 @@
       <c r="C1" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="148" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="148" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="148" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="130">
-        <v>7.6580000000000004</v>
+      <c r="A2" s="131">
+        <v>7.4809999999999999</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>7.6580000000000004</v>
-      </c>
-      <c r="D2">
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>7.4809999999999999</v>
+      </c>
+      <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>46.448999999999998</v>
-      </c>
-      <c r="E2" s="52" t="s">
+        <v>42.224999999999994</v>
+      </c>
+      <c r="E2" s="147" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="149">
         <f>'Charge XX'!F4</f>
-        <v>46.445</v>
+        <v>42.222000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>7.7149999999999999</v>
+        <v>7.7910000000000004</v>
       </c>
       <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>7.7149999999999999</v>
-      </c>
-      <c r="E3" s="52" t="s">
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>7.7910000000000004</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="147" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="149">
         <f>SUM(C:C)</f>
-        <v>46.448999999999998</v>
+        <v>42.224999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="131">
-        <v>8.9570000000000007</v>
+        <v>8.5909999999999993</v>
       </c>
       <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>8.9570000000000007</v>
-      </c>
-      <c r="E4" s="52" t="s">
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>8.5909999999999993</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="149">
         <f>F3-F2</f>
-        <v>3.9999999999977831E-3</v>
+        <v>2.9999999999930083E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>9.6129999999999995</v>
+        <v>5.1639999999999997</v>
       </c>
       <c r="B5" s="130">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>9.6129999999999995</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>5.1639999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="131">
-        <v>12.506</v>
+        <v>6.0380000000000003</v>
       </c>
       <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>12.506</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>6.0380000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>5.4930000000000003</v>
+        <v>7.16</v>
       </c>
       <c r="B7" s="130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>7.16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="131">
-        <v>5.6980000000000004</v>
+        <v>6.2480000000000002</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>7.7910000000000004</v>
+        <v>6.3310000000000004</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="131">
-        <v>7.8949999999999996</v>
+      <c r="A10" s="130">
+        <v>6.8639999999999999</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="131">
-        <v>8.5909999999999993</v>
+        <v>6.8949999999999996</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="130">
-        <v>10.977</v>
+      <c r="A12" s="131">
+        <v>7.1429999999999998</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>5.1639999999999997</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="131">
-        <v>6.0380000000000003</v>
+      <c r="A14" s="130">
+        <v>7.7149999999999999</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="131">
-        <v>6.2480000000000002</v>
+        <v>8.9570000000000007</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>6.3310000000000004</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="130">
-        <v>6.8639999999999999</v>
+      <c r="A17" s="131">
+        <v>12.506</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="131">
-        <v>6.8949999999999996</v>
+      <c r="A18" s="130">
+        <v>5.4930000000000003</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="131">
-        <v>6.9009999999999998</v>
+        <v>5.6980000000000004</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="131">
-        <v>7.1429999999999998</v>
+        <v>7.8949999999999996</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>7.16</v>
+        <v>10.977</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="130">
+      <c r="A22" s="131">
+        <v>6.9009999999999998</v>
+      </c>
+      <c r="B22" s="130">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>IF(A22=0, 0, A22*B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="130">
         <v>7.2839999999999998</v>
       </c>
-      <c r="B22" s="130">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="131">
-        <v>7.4809999999999999</v>
-      </c>
       <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -7671,7 +7682,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -7683,7 +7694,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -7693,7 +7704,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -7703,7 +7714,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -7713,7 +7724,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -7723,7 +7734,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -7733,7 +7744,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -7743,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -7753,7 +7764,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -7763,7 +7774,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -7773,7 +7784,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -7783,7 +7794,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -7793,7 +7804,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -7803,7 +7814,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -7813,7 +7824,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -7823,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -7833,7 +7844,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -7843,7 +7854,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -7853,7 +7864,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -7863,7 +7874,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -7873,7 +7884,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -7883,7 +7894,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -7893,7 +7904,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -7903,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -7913,7 +7924,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -7923,7 +7934,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -7933,7 +7944,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -7943,7 +7954,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -7972,8 +7983,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -8002,386 +8013,386 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>18.545999999999999</v>
+        <v>5.5650000000000004</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>18.545999999999999</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>5.5650000000000004</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>57.671999999999997</v>
+        <v>52.415999999999997</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="53">
         <f>'Charge XX'!F5</f>
-        <v>57.664000000000001</v>
+        <v>52.421999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>12.461</v>
+        <v>24.922999999999998</v>
       </c>
       <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>12.461</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>24.922999999999998</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="53">
         <f>SUM(C:C)</f>
-        <v>57.671999999999997</v>
+        <v>52.415999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="130">
-        <v>10.122999999999999</v>
+        <v>21.928000000000001</v>
       </c>
       <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>10.122999999999999</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>21.928000000000001</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>7.9999999999955662E-3</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>6.6609999999999996</v>
+        <v>4.3159999999999998</v>
       </c>
       <c r="B5" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>6.6609999999999996</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>5.5650000000000004</v>
+        <v>25.873000000000001</v>
       </c>
       <c r="B6" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>5.5650000000000004</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>4.3159999999999998</v>
+        <v>20.651</v>
       </c>
       <c r="B7" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>4.3159999999999998</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="130">
-        <v>29.986999999999998</v>
+        <v>23.978999999999999</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>29.632000000000001</v>
+        <v>15.534000000000001</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="130">
-        <v>28.844000000000001</v>
+        <v>6.8360000000000003</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="130">
-        <v>28.742000000000001</v>
+        <v>4.4930000000000003</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="130">
-        <v>28.638000000000002</v>
+        <v>18.545999999999999</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>28.478999999999999</v>
+        <v>12.461</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="130">
-        <v>27.143000000000001</v>
+        <v>10.122999999999999</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="130">
-        <v>25.873000000000001</v>
+        <v>6.6609999999999996</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>25.02</v>
+        <v>29.986999999999998</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="130">
-        <v>24.922999999999998</v>
+        <v>29.632000000000001</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="130">
-        <v>23.978999999999999</v>
+        <v>28.844000000000001</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="130">
-        <v>22.062999999999999</v>
+        <v>28.742000000000001</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="130">
-        <v>21.928000000000001</v>
+        <v>28.638000000000002</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>20.651</v>
+        <v>28.478999999999999</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="130">
-        <v>20.65</v>
+        <v>27.143000000000001</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="130">
-        <v>19.782</v>
+        <v>25.02</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="130">
-        <v>19.518999999999998</v>
+        <v>22.062999999999999</v>
       </c>
       <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="130">
-        <v>19.449000000000002</v>
+        <v>20.65</v>
       </c>
       <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="130">
-        <v>15.534000000000001</v>
+        <v>19.782</v>
       </c>
       <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="130">
-        <v>14.474</v>
+        <v>19.518999999999998</v>
       </c>
       <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="130">
-        <v>11.648999999999999</v>
+        <v>19.449000000000002</v>
       </c>
       <c r="B28" s="130">
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="130">
-        <v>11.284000000000001</v>
+        <v>14.474</v>
       </c>
       <c r="B29" s="130">
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="130">
-        <v>6.8360000000000003</v>
+        <v>11.648999999999999</v>
       </c>
       <c r="B30" s="130">
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="130">
-        <v>4.4930000000000003</v>
+        <v>11.284000000000001</v>
       </c>
       <c r="B31" s="130">
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -8391,7 +8402,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -8401,7 +8412,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -8411,7 +8422,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8421,7 +8432,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -8431,7 +8442,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -8441,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -8451,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8461,7 +8472,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -8471,7 +8482,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -8481,7 +8492,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -8491,7 +8502,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -8501,7 +8512,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -8511,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -8521,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -8531,7 +8542,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -8541,7 +8552,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -8551,7 +8562,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -8561,7 +8572,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -8571,7 +8582,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -8581,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -8610,8 +8621,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -8658,7 +8669,7 @@
       </c>
       <c r="F2" s="53">
         <f>'Charge XX'!F6</f>
-        <v>5.891</v>
+        <v>5.3559999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8696,7 +8707,7 @@
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>-4.1000000000000369E-2</v>
+        <v>0.49399999999999977</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9232,8 +9243,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -9864,8 +9875,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>

</xml_diff>

<commit_message>
Locked main sheet, check box write alloy comp to true values, changed file strucutre
</commit_message>
<xml_diff>
--- a/Prototype - AutoChargeCalcs.xlsx
+++ b/Prototype - AutoChargeCalcs.xlsx
@@ -1332,6 +1332,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1374,14 +1382,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4554,15 +4554,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="137" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -4601,7 +4601,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="64" t="str">
-        <f>A3</f>
+        <f>Q4 &amp; ROUND(N4,3)*100 &amp; Q5 &amp; ROUND(N5,3)*100 &amp; Q6 &amp; ROUND(N6,3)*100 &amp; Q7 &amp; ROUND(N7,3)*100 &amp; Q8 &amp; ROUND(N8,3)*100</f>
         <v>Mg65Zn30Ca5D0E0</v>
       </c>
       <c r="J3" s="65"/>
@@ -4687,19 +4687,19 @@
       <c r="J4" s="28"/>
       <c r="K4" s="74">
         <f>B29</f>
-        <v>42.224999999999994</v>
+        <v>42.216000000000001</v>
       </c>
       <c r="L4" s="75">
         <f>K4/$K$9</f>
-        <v>0.42018688240737978</v>
+        <v>0.42214733557993261</v>
       </c>
       <c r="M4" s="25">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.7288084032395793E-2</v>
+        <v>1.7368744520877704E-2</v>
       </c>
       <c r="N4" s="120">
         <f>M4/$M$9</f>
-        <v>0.64704980052908057</v>
+        <v>0.64986390801406102</v>
       </c>
       <c r="P4" s="17">
         <v>1</v>
@@ -4780,19 +4780,19 @@
       <c r="J5" s="29"/>
       <c r="K5" s="77">
         <f>E29</f>
-        <v>52.415999999999997</v>
+        <v>52.403000000000006</v>
       </c>
       <c r="L5" s="78">
         <f>K5/$K$9</f>
-        <v>0.52159894915962624</v>
+        <v>0.52401427957161295</v>
       </c>
       <c r="M5" s="26">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>7.9777148016216427E-3</v>
+        <v>8.014656626772091E-3</v>
       </c>
       <c r="N5" s="121">
         <f>M5/$M$9</f>
-        <v>0.29858593707632664</v>
+        <v>0.29987406807695405</v>
       </c>
       <c r="P5" s="17">
         <v>2</v>
@@ -4873,19 +4873,19 @@
       <c r="J6" s="29"/>
       <c r="K6" s="79">
         <f>H29</f>
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="L6" s="78">
         <f>K6/$K$9</f>
-        <v>5.8214168432994005E-2</v>
+        <v>5.3838384848454553E-2</v>
       </c>
       <c r="M6" s="26">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.4525217933278607E-3</v>
+        <v>1.3433401080007621E-3</v>
       </c>
       <c r="N6" s="121">
         <f>M6/$M$9</f>
-        <v>5.4364262394592786E-2</v>
+        <v>5.0262023908984925E-2</v>
       </c>
       <c r="P6" s="17">
         <v>3</v>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="K9" s="122">
         <f>SUM(K4:K8)</f>
-        <v>100.49099999999999</v>
+        <v>100.003</v>
       </c>
       <c r="L9" s="86">
         <f>SUM(L4:L8)</f>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="M9" s="123">
         <f>SUM(M4:M8)</f>
-        <v>2.6718320627345298E-2</v>
+        <v>2.6726741255650558E-2</v>
       </c>
       <c r="N9" s="87">
         <f>SUM(N4:N8)</f>
@@ -5197,35 +5197,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="137" t="str">
+      <c r="A12" s="141" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="138"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="139" t="str">
+      <c r="D12" s="143" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="140"/>
+      <c r="E12" s="144"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="141" t="str">
+      <c r="G12" s="145" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="142"/>
+      <c r="H12" s="146"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="143" t="str">
+      <c r="J12" s="147" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="144"/>
+      <c r="K12" s="148"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="145" t="str">
+      <c r="M12" s="149" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="146"/>
+      <c r="N12" s="150"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="B14" s="110">
         <f>A!C2</f>
-        <v>7.4809999999999999</v>
+        <v>7.16</v>
       </c>
       <c r="C14" s="111"/>
       <c r="D14" s="132">
@@ -5299,7 +5299,7 @@
       </c>
       <c r="E14" s="110">
         <f>B!C2</f>
-        <v>5.5650000000000004</v>
+        <v>4.3159999999999998</v>
       </c>
       <c r="F14" s="111"/>
       <c r="G14" s="132">
@@ -5307,7 +5307,7 @@
       </c>
       <c r="H14" s="110">
         <f>'C'!C2</f>
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="I14" s="111"/>
       <c r="J14" s="132">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="B15" s="110">
         <f>A!C3</f>
-        <v>7.7910000000000004</v>
+        <v>7.8949999999999996</v>
       </c>
       <c r="C15" s="111"/>
       <c r="D15" s="132">
@@ -5349,7 +5349,7 @@
       </c>
       <c r="E15" s="110">
         <f>B!C3</f>
-        <v>24.922999999999998</v>
+        <v>19.449000000000002</v>
       </c>
       <c r="F15" s="111"/>
       <c r="G15" s="132">
@@ -5399,7 +5399,7 @@
       </c>
       <c r="E16" s="110">
         <f>B!C4</f>
-        <v>21.928000000000001</v>
+        <v>28.638000000000002</v>
       </c>
       <c r="F16" s="111"/>
       <c r="G16" s="132">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="B17" s="110">
         <f>A!C5</f>
-        <v>5.1639999999999997</v>
+        <v>8.9570000000000007</v>
       </c>
       <c r="C17" s="111"/>
       <c r="D17" s="132">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="B18" s="110">
         <f>A!C6</f>
-        <v>6.0380000000000003</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="C18" s="111"/>
       <c r="D18" s="132">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B19" s="110">
         <f>A!C7</f>
-        <v>7.16</v>
+        <v>0</v>
       </c>
       <c r="C19" s="111"/>
       <c r="D19" s="132">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="B29" s="114">
         <f>SUM(B14:B28)</f>
-        <v>42.224999999999994</v>
+        <v>42.216000000000001</v>
       </c>
       <c r="C29" s="111"/>
       <c r="D29" s="113" t="s">
@@ -5989,7 +5989,7 @@
       </c>
       <c r="E29" s="115">
         <f>SUM(E14:E28)</f>
-        <v>52.415999999999997</v>
+        <v>52.403000000000006</v>
       </c>
       <c r="F29" s="111"/>
       <c r="G29" s="113" t="s">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H29" s="114">
         <f>SUM(H14:H28)</f>
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="I29" s="111"/>
       <c r="J29" s="113" t="s">
@@ -6022,7 +6022,7 @@
       </c>
       <c r="B30" s="117">
         <f>B29-$F$4</f>
-        <v>2.9999999999930083E-3</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
       <c r="C30" s="118"/>
       <c r="D30" s="116" t="s">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="E30" s="117">
         <f>E29-$F$5</f>
-        <v>-6.0000000000002274E-3</v>
+        <v>-1.8999999999991246E-2</v>
       </c>
       <c r="F30" s="118"/>
       <c r="G30" s="116" t="s">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="H30" s="117">
         <f>H29-$F$6</f>
-        <v>0.49399999999999977</v>
+        <v>2.8000000000000469E-2</v>
       </c>
       <c r="I30" s="118"/>
       <c r="J30" s="116" t="s">
@@ -6059,35 +6059,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="134" t="s">
+      <c r="A32" s="138" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="135"/>
-      <c r="C32" s="135"/>
-      <c r="D32" s="135"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="135"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="135"/>
-      <c r="I32" s="135"/>
-      <c r="J32" s="135"/>
-      <c r="K32" s="135"/>
-      <c r="L32" s="135"/>
-      <c r="M32" s="135"/>
-      <c r="N32" s="135"/>
-      <c r="O32" s="135"/>
-      <c r="P32" s="135"/>
-      <c r="Q32" s="135"/>
-      <c r="R32" s="135"/>
-      <c r="S32" s="135"/>
-      <c r="T32" s="135"/>
-      <c r="U32" s="135"/>
-      <c r="V32" s="135"/>
-      <c r="W32" s="135"/>
-      <c r="X32" s="135"/>
-      <c r="Y32" s="135"/>
-      <c r="Z32" s="135"/>
-      <c r="AA32" s="136"/>
+      <c r="B32" s="139"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="139"/>
+      <c r="I32" s="139"/>
+      <c r="J32" s="139"/>
+      <c r="K32" s="139"/>
+      <c r="L32" s="139"/>
+      <c r="M32" s="139"/>
+      <c r="N32" s="139"/>
+      <c r="O32" s="139"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="139"/>
+      <c r="R32" s="139"/>
+      <c r="S32" s="139"/>
+      <c r="T32" s="139"/>
+      <c r="U32" s="139"/>
+      <c r="V32" s="139"/>
+      <c r="W32" s="139"/>
+      <c r="X32" s="139"/>
+      <c r="Y32" s="139"/>
+      <c r="Z32" s="139"/>
+      <c r="AA32" s="140"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -7327,6 +7327,7 @@
     <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A32:AA32"/>
@@ -7350,13 +7351,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -7373,57 +7374,57 @@
       <c r="C1" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="148" t="s">
+      <c r="D1" s="134" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="148" t="s">
+      <c r="E1" s="134" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="148" t="s">
+      <c r="F1" s="134" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="131">
-        <v>7.4809999999999999</v>
+      <c r="A2" s="130">
+        <v>7.16</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>7.4809999999999999</v>
+        <v>7.16</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>42.224999999999994</v>
-      </c>
-      <c r="E2" s="147" t="s">
+        <v>42.216000000000001</v>
+      </c>
+      <c r="E2" s="133" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="149">
+      <c r="F2" s="135">
         <f>'Charge XX'!F4</f>
         <v>42.222000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="130">
-        <v>7.7910000000000004</v>
+      <c r="A3" s="131">
+        <v>7.8949999999999996</v>
       </c>
       <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
         <f>IF(A3=0, 0, A3*B3)</f>
-        <v>7.7910000000000004</v>
+        <v>7.8949999999999996</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="133" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="149">
+      <c r="F3" s="135">
         <f>SUM(C:C)</f>
-        <v>42.224999999999994</v>
+        <v>42.216000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7438,53 +7439,53 @@
         <v>8.5909999999999993</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="147" t="s">
+      <c r="E4" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="149">
+      <c r="F4" s="135">
         <f>F3-F2</f>
-        <v>2.9999999999930083E-3</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="130">
-        <v>5.1639999999999997</v>
+      <c r="A5" s="131">
+        <v>8.9570000000000007</v>
       </c>
       <c r="B5" s="130">
         <v>1</v>
       </c>
       <c r="C5">
         <f>IF(A5=0, 0, A5*B5)</f>
-        <v>5.1639999999999997</v>
+        <v>8.9570000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="131">
-        <v>6.0380000000000003</v>
+      <c r="A6" s="130">
+        <v>9.6129999999999995</v>
       </c>
       <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
         <f>IF(A6=0, 0, A6*B6)</f>
-        <v>6.0380000000000003</v>
+        <v>9.6129999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>7.16</v>
+        <v>5.1639999999999997</v>
       </c>
       <c r="B7" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>IF(A7=0, 0, A7*B7)</f>
-        <v>7.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="131">
-        <v>6.2480000000000002</v>
+      <c r="A8" s="130">
+        <v>5.4930000000000003</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
@@ -7495,8 +7496,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="130">
-        <v>6.3310000000000004</v>
+      <c r="A9" s="131">
+        <v>5.6980000000000004</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
@@ -7507,8 +7508,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="130">
-        <v>6.8639999999999999</v>
+      <c r="A10" s="131">
+        <v>6.0380000000000003</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
@@ -7520,7 +7521,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="131">
-        <v>6.8949999999999996</v>
+        <v>6.2480000000000002</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
@@ -7531,8 +7532,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="131">
-        <v>7.1429999999999998</v>
+      <c r="A12" s="130">
+        <v>6.3310000000000004</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
@@ -7544,7 +7545,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>7.6580000000000004</v>
+        <v>6.8639999999999999</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
@@ -7555,8 +7556,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="130">
-        <v>7.7149999999999999</v>
+      <c r="A14" s="131">
+        <v>6.8949999999999996</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
@@ -7568,7 +7569,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="131">
-        <v>8.9570000000000007</v>
+        <v>6.9009999999999998</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
@@ -7579,8 +7580,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="130">
-        <v>9.6129999999999995</v>
+      <c r="A16" s="131">
+        <v>7.1429999999999998</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
@@ -7591,8 +7592,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="131">
-        <v>12.506</v>
+      <c r="A17" s="130">
+        <v>7.2839999999999998</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
@@ -7603,8 +7604,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="130">
-        <v>5.4930000000000003</v>
+      <c r="A18" s="131">
+        <v>7.4809999999999999</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
@@ -7615,8 +7616,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="131">
-        <v>5.6980000000000004</v>
+      <c r="A19" s="130">
+        <v>7.6580000000000004</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
@@ -7627,8 +7628,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="131">
-        <v>7.8949999999999996</v>
+      <c r="A20" s="130">
+        <v>7.7149999999999999</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
@@ -7640,7 +7641,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>10.977</v>
+        <v>7.7910000000000004</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
@@ -7651,8 +7652,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="131">
-        <v>6.9009999999999998</v>
+      <c r="A22" s="130">
+        <v>8.6839999999999993</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
@@ -7663,8 +7664,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="130">
-        <v>7.2839999999999998</v>
+      <c r="A23" s="131">
+        <v>8.9120000000000008</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
@@ -7676,7 +7677,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="130">
-        <v>8.6839999999999993</v>
+        <v>10.977</v>
       </c>
       <c r="B24" s="130">
         <v>0</v>
@@ -7688,7 +7689,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="131">
-        <v>8.9120000000000008</v>
+        <v>12.506</v>
       </c>
       <c r="B25" s="130">
         <v>0</v>
@@ -7978,13 +7979,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -8013,18 +8014,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>5.5650000000000004</v>
+        <v>4.3159999999999998</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>5.5650000000000004</v>
+        <v>4.3159999999999998</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>52.415999999999997</v>
+        <v>52.403000000000006</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>109</v>
@@ -8036,45 +8037,45 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>24.922999999999998</v>
+        <v>19.449000000000002</v>
       </c>
       <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
         <f>IF(A3=0, 0, A3*B3)</f>
-        <v>24.922999999999998</v>
+        <v>19.449000000000002</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="53">
         <f>SUM(C:C)</f>
-        <v>52.415999999999997</v>
+        <v>52.403000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="130">
-        <v>21.928000000000001</v>
+        <v>28.638000000000002</v>
       </c>
       <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
         <f>IF(A4=0, 0, A4*B4)</f>
-        <v>21.928000000000001</v>
+        <v>28.638000000000002</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>-6.0000000000002274E-3</v>
+        <v>-1.8999999999991246E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>4.3159999999999998</v>
+        <v>15.534000000000001</v>
       </c>
       <c r="B5" s="130">
         <v>0</v>
@@ -8086,7 +8087,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>25.873000000000001</v>
+        <v>4.4930000000000003</v>
       </c>
       <c r="B6" s="130">
         <v>0</v>
@@ -8098,7 +8099,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>20.651</v>
+        <v>5.5650000000000004</v>
       </c>
       <c r="B7" s="130">
         <v>0</v>
@@ -8110,7 +8111,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="130">
-        <v>23.978999999999999</v>
+        <v>6.6609999999999996</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
@@ -8122,7 +8123,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>15.534000000000001</v>
+        <v>6.8360000000000003</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
@@ -8134,7 +8135,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="130">
-        <v>6.8360000000000003</v>
+        <v>10.122999999999999</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
@@ -8146,7 +8147,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="130">
-        <v>4.4930000000000003</v>
+        <v>11.284000000000001</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
@@ -8158,7 +8159,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="130">
-        <v>18.545999999999999</v>
+        <v>11.648999999999999</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
@@ -8182,7 +8183,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="130">
-        <v>10.122999999999999</v>
+        <v>14.474</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
@@ -8194,7 +8195,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="130">
-        <v>6.6609999999999996</v>
+        <v>18.545999999999999</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
@@ -8206,7 +8207,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>29.986999999999998</v>
+        <v>19.518999999999998</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
@@ -8218,7 +8219,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="130">
-        <v>29.632000000000001</v>
+        <v>19.782</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
@@ -8230,7 +8231,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="130">
-        <v>28.844000000000001</v>
+        <v>20.65</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
@@ -8242,7 +8243,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="130">
-        <v>28.742000000000001</v>
+        <v>20.651</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
@@ -8254,7 +8255,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="130">
-        <v>28.638000000000002</v>
+        <v>21.928000000000001</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
@@ -8266,7 +8267,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>28.478999999999999</v>
+        <v>22.062999999999999</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
@@ -8278,7 +8279,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="130">
-        <v>27.143000000000001</v>
+        <v>23.978999999999999</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
@@ -8290,7 +8291,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="130">
-        <v>25.02</v>
+        <v>24.922999999999998</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
@@ -8302,7 +8303,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="130">
-        <v>22.062999999999999</v>
+        <v>25.02</v>
       </c>
       <c r="B24" s="130">
         <v>0</v>
@@ -8314,7 +8315,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="130">
-        <v>20.65</v>
+        <v>25.873000000000001</v>
       </c>
       <c r="B25" s="130">
         <v>0</v>
@@ -8326,7 +8327,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="130">
-        <v>19.782</v>
+        <v>27.143000000000001</v>
       </c>
       <c r="B26" s="130">
         <v>0</v>
@@ -8338,7 +8339,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="130">
-        <v>19.518999999999998</v>
+        <v>28.478999999999999</v>
       </c>
       <c r="B27" s="130">
         <v>0</v>
@@ -8350,7 +8351,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="130">
-        <v>19.449000000000002</v>
+        <v>28.742000000000001</v>
       </c>
       <c r="B28" s="130">
         <v>0</v>
@@ -8362,7 +8363,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="130">
-        <v>14.474</v>
+        <v>28.844000000000001</v>
       </c>
       <c r="B29" s="130">
         <v>0</v>
@@ -8374,7 +8375,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="130">
-        <v>11.648999999999999</v>
+        <v>29.632000000000001</v>
       </c>
       <c r="B30" s="130">
         <v>0</v>
@@ -8386,7 +8387,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="130">
-        <v>11.284000000000001</v>
+        <v>29.986999999999998</v>
       </c>
       <c r="B31" s="130">
         <v>0</v>
@@ -8616,13 +8617,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -8651,18 +8652,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>5.85</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>5.3840000000000003</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>109</v>
@@ -8674,13 +8675,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>9.593</v>
+        <v>0.42149999999999999</v>
       </c>
       <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -8688,18 +8689,18 @@
       </c>
       <c r="F3" s="53">
         <f>SUM(C:C)</f>
-        <v>5.85</v>
+        <v>5.3840000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="130">
-        <v>9.4710000000000001</v>
+        <v>2.4849999999999999</v>
       </c>
       <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -8707,234 +8708,234 @@
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>0.49399999999999977</v>
+        <v>2.8000000000000469E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>9.2479999999999993</v>
+        <v>3.2149999999999999</v>
       </c>
       <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>8.4350000000000005</v>
+        <v>3.9380000000000002</v>
       </c>
       <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>7.6950000000000003</v>
+        <v>4.1280000000000001</v>
       </c>
       <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="130">
-        <v>7.4480000000000004</v>
+        <v>4.165</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>6.9880000000000004</v>
+        <v>4.2690000000000001</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="130">
-        <v>6.7270000000000003</v>
+        <v>4.7759999999999998</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="130">
-        <v>5.5860000000000003</v>
+        <v>4.923</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="130">
-        <v>5.5129999999999999</v>
+        <v>5.2220000000000004</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>5.3840000000000003</v>
+        <v>5.5129999999999999</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="130">
-        <v>5.2220000000000004</v>
+        <v>5.5860000000000003</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="130">
-        <v>4.923</v>
+        <v>5.85</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>4.7759999999999998</v>
+        <v>6.7270000000000003</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="130">
-        <v>4.2690000000000001</v>
+        <v>6.9880000000000004</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="130">
-        <v>4.165</v>
+        <v>7.4480000000000004</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="130">
-        <v>4.1280000000000001</v>
+        <v>7.6950000000000003</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="130">
-        <v>3.9380000000000002</v>
+        <v>8.4350000000000005</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>2.4849999999999999</v>
+        <v>9.2479999999999993</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="130">
-        <v>3.2149999999999999</v>
+        <v>9.4710000000000001</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="130">
-        <v>0.42149999999999999</v>
+        <v>9.593</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8944,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -8954,7 +8955,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -8964,7 +8965,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -8974,7 +8975,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -8984,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -8994,7 +8995,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -9004,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -9014,7 +9015,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -9024,7 +9025,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -9034,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -9044,7 +9045,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9054,7 +9055,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -9064,7 +9065,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9074,7 +9075,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -9084,7 +9085,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -9094,7 +9095,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -9104,7 +9105,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -9114,7 +9115,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -9124,7 +9125,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -9134,7 +9135,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -9144,7 +9145,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -9154,7 +9155,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -9164,7 +9165,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -9174,7 +9175,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -9184,7 +9185,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -9194,7 +9195,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -9204,7 +9205,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9214,7 +9215,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -9243,8 +9244,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -9273,7 +9274,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>9.1289999999999996</v>
+        <v>3.4380000000000002</v>
       </c>
       <c r="B2" s="130">
         <v>0</v>
@@ -9296,13 +9297,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>0.16300000000000001</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C51" si="0">IF(A3=0, 0, A3*B3)</f>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -9315,13 +9316,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="130">
-        <v>1.71</v>
+        <v>1.746</v>
       </c>
       <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -9334,277 +9335,277 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>3.4380000000000002</v>
+        <v>7.5640000000000001</v>
       </c>
       <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>0.35299999999999998</v>
+        <v>4.22</v>
       </c>
       <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>1.746</v>
+        <v>3.55</v>
       </c>
       <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="130">
-        <v>7.5640000000000001</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>9.3130000000000006</v>
+        <v>0.185</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="130">
-        <v>4.22</v>
+        <v>0.184</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="130">
-        <v>3.55</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="130">
-        <v>0.67800000000000005</v>
+        <v>7.2069999999999999</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>2.1190000000000002</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="130">
-        <v>0.106</v>
+        <v>2.1269999999999998</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="130">
-        <v>0.185</v>
+        <v>9.1289999999999996</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>5.9859999999999998</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="130">
-        <v>0.184</v>
+        <v>1.71</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="130">
-        <v>1.6379999999999999</v>
+        <v>9.3130000000000006</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="130">
-        <v>7.2069999999999999</v>
+        <v>2.1190000000000002</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="130">
-        <v>2.1840000000000002</v>
+        <v>0.106</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>1.2290000000000001</v>
+        <v>5.9859999999999998</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="130">
-        <v>0.79400000000000004</v>
+        <v>2.1840000000000002</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="130">
-        <v>8.4559999999999995</v>
+        <v>1.2290000000000001</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="130">
-        <v>8.8759999999999994</v>
+        <v>8.4559999999999995</v>
       </c>
       <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="130">
-        <v>9.8610000000000007</v>
+        <v>8.8759999999999994</v>
       </c>
       <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="130">
-        <v>8.5350000000000001</v>
+        <v>9.8610000000000007</v>
       </c>
       <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="130">
-        <v>2.1269999999999998</v>
+        <v>8.5350000000000001</v>
       </c>
       <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -9616,7 +9617,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -9626,7 +9627,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -9636,7 +9637,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -9646,7 +9647,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -9656,7 +9657,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -9666,7 +9667,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -9676,7 +9677,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9686,7 +9687,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -9696,7 +9697,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9706,7 +9707,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -9716,7 +9717,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -9726,7 +9727,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -9736,7 +9737,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -9746,7 +9747,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -9756,7 +9757,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -9766,7 +9767,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -9776,7 +9777,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -9786,7 +9787,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -9796,7 +9797,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -9806,7 +9807,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -9816,7 +9817,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -9826,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -9836,7 +9837,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9846,7 +9847,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -9875,8 +9876,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="150" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="150" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
@@ -9905,7 +9906,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>4.1269999999999998</v>
+        <v>3.8090000000000002</v>
       </c>
       <c r="B2" s="130">
         <v>0</v>
@@ -9928,13 +9929,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="130">
-        <v>5.1159999999999997</v>
+        <v>7.85</v>
       </c>
       <c r="B3" s="130">
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C51" si="0">IF(A3=0, 0, A3*B3)</f>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -9947,13 +9948,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="130">
-        <v>5.7830000000000004</v>
+        <v>3.2509999999999999</v>
       </c>
       <c r="B4" s="130">
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -9966,277 +9967,277 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>2.669</v>
+        <v>7.851</v>
       </c>
       <c r="B5" s="130">
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>6.3630000000000004</v>
+        <v>4.1269999999999998</v>
       </c>
       <c r="B6" s="130">
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>1.627</v>
+        <v>5.1159999999999997</v>
       </c>
       <c r="B7" s="130">
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="130">
-        <v>2.1080000000000001</v>
+        <v>5.7830000000000004</v>
       </c>
       <c r="B8" s="130">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="130">
-        <v>1.4119999999999999</v>
+        <v>2.669</v>
       </c>
       <c r="B9" s="130">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="130">
-        <v>8.0530000000000008</v>
+        <v>6.3630000000000004</v>
       </c>
       <c r="B10" s="130">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="130">
-        <v>3.8090000000000002</v>
+        <v>1.627</v>
       </c>
       <c r="B11" s="130">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="130">
-        <v>2.6139999999999999</v>
+        <v>2.1080000000000001</v>
       </c>
       <c r="B12" s="130">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="130">
-        <v>3.5190000000000001</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="B13" s="130">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="130">
-        <v>8.4550000000000001</v>
+        <v>8.0530000000000008</v>
       </c>
       <c r="B14" s="130">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="130">
-        <v>5.8879999999999999</v>
+        <v>2.6139999999999999</v>
       </c>
       <c r="B15" s="130">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="130">
-        <v>8.1110000000000007</v>
+        <v>3.5190000000000001</v>
       </c>
       <c r="B16" s="130">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="130">
-        <v>5.0190000000000001</v>
+        <v>8.4550000000000001</v>
       </c>
       <c r="B17" s="130">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="130">
-        <v>7.85</v>
+        <v>5.8879999999999999</v>
       </c>
       <c r="B18" s="130">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="130">
-        <v>4.3769999999999998</v>
+        <v>8.1110000000000007</v>
       </c>
       <c r="B19" s="130">
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="130">
-        <v>6.49</v>
+        <v>5.0190000000000001</v>
       </c>
       <c r="B20" s="130">
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="130">
-        <v>7.4050000000000002</v>
+        <v>4.3769999999999998</v>
       </c>
       <c r="B21" s="130">
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="130">
-        <v>2.8319999999999999</v>
+        <v>6.49</v>
       </c>
       <c r="B22" s="130">
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="130">
-        <v>3.2509999999999999</v>
+        <v>7.4050000000000002</v>
       </c>
       <c r="B23" s="130">
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="130">
-        <v>3.2069999999999999</v>
+        <v>2.8319999999999999</v>
       </c>
       <c r="B24" s="130">
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="130">
-        <v>8.4109999999999996</v>
+        <v>3.2069999999999999</v>
       </c>
       <c r="B25" s="130">
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="130">
-        <v>4.9119999999999999</v>
+        <v>8.4109999999999996</v>
       </c>
       <c r="B26" s="130">
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="130">
-        <v>7.851</v>
+        <v>4.9119999999999999</v>
       </c>
       <c r="B27" s="130">
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -10248,7 +10249,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -10258,7 +10259,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -10268,7 +10269,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -10278,7 +10279,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -10288,7 +10289,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -10298,7 +10299,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -10308,7 +10309,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -10318,7 +10319,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -10328,7 +10329,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -10338,7 +10339,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -10348,7 +10349,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -10358,7 +10359,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -10368,7 +10369,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -10378,7 +10379,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -10388,7 +10389,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -10398,7 +10399,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -10408,7 +10409,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -10418,7 +10419,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -10428,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -10438,7 +10439,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -10448,7 +10449,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -10458,7 +10459,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -10468,7 +10469,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -10478,7 +10479,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>